<commit_message>
more space in calendar area
</commit_message>
<xml_diff>
--- a/calendar-2020/calendar-2020.xlsx
+++ b/calendar-2020/calendar-2020.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\GitHub\calendars\calendar-2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7351A06-B240-4E68-AE25-0F261E034135}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B56A81-6CE1-44D5-BF14-4F3ABFBC72A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6B5A2DB5-5F90-46CE-8756-FCA2FB69F658}"/>
   </bookViews>
@@ -504,7 +504,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.21875" customWidth="1"/>
-    <col min="2" max="2" width="3.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="4.44140625" style="4" customWidth="1"/>
     <col min="3" max="39" width="3.33203125" style="1" customWidth="1"/>
     <col min="40" max="40" width="2.21875" customWidth="1"/>
   </cols>

</xml_diff>